<commit_message>
se finaliza lab03 con Edvin Paiz
se termina lab
</commit_message>
<xml_diff>
--- a/Lab03/PINOUT LAB03.xlsx
+++ b/Lab03/PINOUT LAB03.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Angie 2026\Electrónica Digital 2\Lab03\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\Digital02\Lab03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA8471C-7A2B-4C25-8F66-3DB23CA3C36E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC294FEC-7914-4D62-AF3B-325ADE33ABF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{38CA4A19-C4A4-B443-AA8F-BED2C3120EBF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="78">
   <si>
     <t>D13</t>
   </si>
@@ -268,6 +268,9 @@
   </si>
   <si>
     <t>D0</t>
+  </si>
+  <si>
+    <t>MASTER</t>
   </si>
 </sst>
 </file>
@@ -428,35 +431,35 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -866,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D50DAB75-1D4A-1F4B-BA8C-006C9BBD0D11}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="105" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -882,66 +885,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="22"/>
       <c r="C1">
         <v>23294</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
     </row>
     <row r="3" spans="1:13" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
     </row>
     <row r="4" spans="1:13" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
     </row>
     <row r="5" spans="1:13" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D6" s="22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D7" s="22"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D8" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
       <c r="K8" s="5" t="s">
         <v>52</v>
       </c>
@@ -977,10 +988,10 @@
         <v>55</v>
       </c>
       <c r="D10" s="3"/>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="22"/>
+      <c r="F10" s="16"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2" t="s">
@@ -997,15 +1008,15 @@
       <c r="A11" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="15"/>
+      <c r="C11" s="20"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="23"/>
+      <c r="F11" s="17"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2" t="s">
@@ -1020,10 +1031,10 @@
       <c r="A12" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="15"/>
+      <c r="C12" s="20"/>
       <c r="D12" s="8"/>
       <c r="E12" s="2" t="s">
         <v>29</v>
@@ -1048,10 +1059,10 @@
       <c r="A13" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="15"/>
+      <c r="C13" s="20"/>
       <c r="D13" s="8"/>
       <c r="E13" s="2" t="s">
         <v>30</v>
@@ -1099,10 +1110,10 @@
       <c r="A15" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="15"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="8"/>
       <c r="E15" s="2" t="s">
         <v>32</v>
@@ -1126,10 +1137,10 @@
       <c r="A16" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="15"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="7"/>
       <c r="E16" s="2" t="s">
         <v>33</v>
@@ -1153,10 +1164,10 @@
       <c r="A17" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="15"/>
+      <c r="C17" s="20"/>
       <c r="D17" s="7" t="s">
         <v>72</v>
       </c>
@@ -1182,10 +1193,10 @@
       <c r="A18" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="15"/>
+      <c r="C18" s="20"/>
       <c r="D18" s="3"/>
       <c r="E18" s="2" t="s">
         <v>35</v>
@@ -1209,10 +1220,10 @@
       <c r="A19" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="15"/>
+      <c r="C19" s="20"/>
       <c r="D19" s="3"/>
       <c r="E19" s="2" t="s">
         <v>36</v>
@@ -1236,31 +1247,31 @@
       <c r="A20" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="15"/>
+      <c r="C20" s="20"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="18"/>
+      <c r="F20" s="19"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="17" t="s">
+      <c r="I20" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="J20" s="17"/>
+      <c r="J20" s="18"/>
       <c r="K20" s="3"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="C21" s="15"/>
+      <c r="C21" s="20"/>
       <c r="D21" s="3"/>
       <c r="E21" s="4" t="s">
         <v>43</v>
@@ -1282,15 +1293,15 @@
       <c r="A22" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="C22" s="15"/>
+      <c r="C22" s="20"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="17" t="s">
+      <c r="E22" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F22" s="17"/>
+      <c r="F22" s="18"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2" t="s">
@@ -1306,15 +1317,15 @@
       <c r="A23" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="15"/>
+      <c r="C23" s="20"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="19" t="s">
+      <c r="E23" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="F23" s="19"/>
+      <c r="F23" s="21"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2" t="s">
@@ -1329,10 +1340,10 @@
       <c r="A24" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="15"/>
+      <c r="C24" s="20"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
@@ -1344,71 +1355,58 @@
       <c r="A25" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="15"/>
+      <c r="C25" s="20"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="15"/>
+      <c r="C26" s="20"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="15"/>
+      <c r="C27" s="20"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="C28" s="15"/>
+      <c r="C28" s="20"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="C29" s="15"/>
+      <c r="C29" s="20"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="15"/>
+      <c r="C30" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="D2:K5"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E22:F22"/>
+  <mergeCells count="30">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B24:C24"/>
@@ -1425,6 +1423,20 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B17:C17"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="D2:K5"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="D6:D7"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>